<commit_message>
feat:Se crea funcion newElementBot , newElement y se agrgan nuevos stilos
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="123">
   <si>
     <t>request</t>
   </si>
@@ -55,6 +55,15 @@
     <t>ey</t>
   </si>
   <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Hola</t>
+  </si>
+  <si>
+    <t>Oe</t>
+  </si>
+  <si>
     <t xml:space="preserve">adios </t>
   </si>
   <si>
@@ -70,58 +79,307 @@
     <t>ten buen día</t>
   </si>
   <si>
+    <t>bye</t>
+  </si>
+  <si>
+    <t>Suerte</t>
+  </si>
+  <si>
+    <t>adíos</t>
+  </si>
+  <si>
+    <t>Adios</t>
+  </si>
+  <si>
     <t>cómo estas</t>
   </si>
   <si>
-    <t>bien y tu</t>
+    <t>Bien gracias por preguntar, en que te puedo ayudar</t>
   </si>
   <si>
     <t>¿cómo estás?</t>
   </si>
   <si>
-    <t>¿cuentame tu día ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">estuvo bien y el tuyo </t>
-  </si>
-  <si>
     <t>cómo estás?</t>
   </si>
   <si>
+    <t xml:space="preserve">¿Cómo estás? </t>
+  </si>
+  <si>
     <t>como estas</t>
   </si>
   <si>
-    <t>bye</t>
+    <t>como vas?</t>
+  </si>
+  <si>
+    <t>como vas</t>
   </si>
   <si>
     <t>¿Quién eres?</t>
   </si>
   <si>
-    <t>Hola soy bot tu asistente virtual</t>
+    <t>Hola soy robotina tu asistente virtual</t>
   </si>
   <si>
     <t>¿Qué haces?</t>
   </si>
   <si>
-    <t>Te leo</t>
+    <t>Estoy disponible para lo que necesites</t>
   </si>
   <si>
     <t xml:space="preserve">¿Cómo te llamas? </t>
   </si>
   <si>
-    <t xml:space="preserve">Hola soy bot </t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Cómo estás? </t>
+    <t>Hola soy robotina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cómo te llamas? </t>
+  </si>
+  <si>
+    <t>Cómo te llamas</t>
+  </si>
+  <si>
+    <t>como te llamas</t>
+  </si>
+  <si>
+    <t>cómo te llamas</t>
+  </si>
+  <si>
+    <t>Cómo funciona</t>
+  </si>
+  <si>
+    <t>Solo dime que necesitas</t>
+  </si>
+  <si>
+    <t>como funciona</t>
+  </si>
+  <si>
+    <t>cmo funciona</t>
+  </si>
+  <si>
+    <t>como funciona?</t>
+  </si>
+  <si>
+    <t>cómo funciona</t>
+  </si>
+  <si>
+    <t>comó funciona</t>
   </si>
   <si>
     <t xml:space="preserve">¿Cómo funciona? </t>
   </si>
   <si>
-    <t>Solo debes decirme que necesitas</t>
-  </si>
-  <si>
     <t>Como estas</t>
+  </si>
+  <si>
+    <t>Que necesitas que funcione</t>
+  </si>
+  <si>
+    <t>¿Que mas?</t>
+  </si>
+  <si>
+    <t>Que mas</t>
+  </si>
+  <si>
+    <t>¿Me puedes ayudar?</t>
+  </si>
+  <si>
+    <t>en que puedo ayudarte</t>
+  </si>
+  <si>
+    <t>Me puedes ayudar</t>
+  </si>
+  <si>
+    <t>Gracias por la ayuda</t>
+  </si>
+  <si>
+    <t>un placer ayudarte</t>
+  </si>
+  <si>
+    <t>tienen productos</t>
+  </si>
+  <si>
+    <t>cuales necesitan</t>
+  </si>
+  <si>
+    <t>cuanto demora si compro con ustedes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">depende de la transportadora </t>
+  </si>
+  <si>
+    <t>tienen descuentos</t>
+  </si>
+  <si>
+    <t>revisa en nuestra campañas</t>
+  </si>
+  <si>
+    <t>hay descuentos</t>
+  </si>
+  <si>
+    <t>donde estan ubicados</t>
+  </si>
+  <si>
+    <t>Medellin, Bogota</t>
+  </si>
+  <si>
+    <t>donde estan ubicados?</t>
+  </si>
+  <si>
+    <t>¿donde estan ubicados?</t>
+  </si>
+  <si>
+    <t>que mas productos tienen</t>
+  </si>
+  <si>
+    <t>todo lo publicamos en nuestra web</t>
+  </si>
+  <si>
+    <t>que mas productos tienen?</t>
+  </si>
+  <si>
+    <t>¿que mas productos tienen?</t>
+  </si>
+  <si>
+    <t>olaaaaa</t>
+  </si>
+  <si>
+    <t>ooooola</t>
+  </si>
+  <si>
+    <t>gracias por la ayuda</t>
+  </si>
+  <si>
+    <t>HooooooolA</t>
+  </si>
+  <si>
+    <t>HOLA</t>
+  </si>
+  <si>
+    <t>Donde estan unbicados</t>
+  </si>
+  <si>
+    <t>DONde estan ubicados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M e puedes ayudar </t>
+  </si>
+  <si>
+    <t>M puedes ayudar</t>
+  </si>
+  <si>
+    <t>comó Funciona</t>
+  </si>
+  <si>
+    <t>como Funciona</t>
+  </si>
+  <si>
+    <t>Que mas productos tienen ?</t>
+  </si>
+  <si>
+    <t>puedo pedir domiciilio</t>
+  </si>
+  <si>
+    <t>nos compartes la direccion</t>
+  </si>
+  <si>
+    <t>Puedo pedir domiciilio</t>
+  </si>
+  <si>
+    <t>Pudo pedir domiciol</t>
+  </si>
+  <si>
+    <t>púedo pedir domicilio</t>
+  </si>
+  <si>
+    <t>Muchas Gracias</t>
+  </si>
+  <si>
+    <t>muchas gracias</t>
+  </si>
+  <si>
+    <t>gracias</t>
+  </si>
+  <si>
+    <t>nos vemos depues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hasta la proxima </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nos vemos Depues </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOS VEMOS DESPUES </t>
+  </si>
+  <si>
+    <t>nos vemos despúes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NBiem gracias </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bien, ¿cuentame en que te puedo ayudar </t>
+  </si>
+  <si>
+    <t>Bien gracias</t>
+  </si>
+  <si>
+    <t>Biencito</t>
+  </si>
+  <si>
+    <t>Biensito</t>
+  </si>
+  <si>
+    <t>biencito</t>
+  </si>
+  <si>
+    <t>biensito</t>
+  </si>
+  <si>
+    <t>Well and you</t>
+  </si>
+  <si>
+    <t>en español por favor</t>
+  </si>
+  <si>
+    <t>robotina</t>
+  </si>
+  <si>
+    <t>Robotina</t>
+  </si>
+  <si>
+    <t>ROBOTINA</t>
+  </si>
+  <si>
+    <t>RoBotINA</t>
+  </si>
+  <si>
+    <t>DBOT</t>
+  </si>
+  <si>
+    <t>Mi nombre es robotina en que puedo ayudarte</t>
+  </si>
+  <si>
+    <t>Bot</t>
+  </si>
+  <si>
+    <t>BOT</t>
+  </si>
+  <si>
+    <t>HASTA LA PRÓXIMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hásta la proxima </t>
+  </si>
+  <si>
+    <t>CHAO</t>
+  </si>
+  <si>
+    <t>CHIAO</t>
+  </si>
+  <si>
+    <t>chiao</t>
   </si>
 </sst>
 </file>
@@ -499,15 +757,15 @@
         <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="17">
@@ -515,15 +773,15 @@
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="19">
@@ -531,7 +789,7 @@
         <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20">
@@ -539,15 +797,15 @@
         <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="22">
@@ -555,36 +813,631 @@
         <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>